<commit_message>
fix: one minute analisis for bnb coins collections
</commit_message>
<xml_diff>
--- a/outputs/excel-coin.xlsx
+++ b/outputs/excel-coin.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <workbookPr codeName="ThisWorkbook"/>
   <sheets>
-    <sheet name="COIN_SECOND" sheetId="1" r:id="rId1"/>
+    <sheet name="COIN_FIRST" sheetId="1" r:id="rId1"/>
   </sheets>
 </workbook>
 </file>
@@ -423,37 +423,37 @@
         <v>0</v>
       </c>
       <c r="B2">
-        <v>7973</v>
+        <v>3960</v>
       </c>
       <c r="C2">
-        <v>5859</v>
+        <v>3371</v>
       </c>
       <c r="D2">
-        <v>5527</v>
+        <v>3626</v>
       </c>
       <c r="E2">
-        <v>5823</v>
+        <v>3336</v>
       </c>
       <c r="F2">
-        <v>5828</v>
+        <v>3147</v>
       </c>
       <c r="G2">
-        <v>5718</v>
+        <v>3274</v>
       </c>
       <c r="H2">
-        <v>5729</v>
+        <v>2934</v>
       </c>
       <c r="I2">
-        <v>5697</v>
+        <v>3248</v>
       </c>
       <c r="J2">
-        <v>5683</v>
+        <v>3447</v>
       </c>
       <c r="K2">
-        <v>5983</v>
+        <v>3360</v>
       </c>
       <c r="L2" t="str">
-        <v>2021-06-22 00:00:00</v>
+        <v>2021-06-24 00:00:00</v>
       </c>
     </row>
     <row r="3">
@@ -461,37 +461,37 @@
         <v>1</v>
       </c>
       <c r="B3">
-        <v>11504</v>
+        <v>7653</v>
       </c>
       <c r="C3">
-        <v>8356</v>
+        <v>6878</v>
       </c>
       <c r="D3">
-        <v>8254</v>
+        <v>7042</v>
       </c>
       <c r="E3">
-        <v>8287</v>
+        <v>6492</v>
       </c>
       <c r="F3">
-        <v>8138</v>
+        <v>6346</v>
       </c>
       <c r="G3">
-        <v>8648</v>
+        <v>6770</v>
       </c>
       <c r="H3">
-        <v>8121</v>
+        <v>6605</v>
       </c>
       <c r="I3">
-        <v>8112</v>
+        <v>6331</v>
       </c>
       <c r="J3">
-        <v>8131</v>
+        <v>6502</v>
       </c>
       <c r="K3">
-        <v>8698</v>
+        <v>6618</v>
       </c>
       <c r="L3" t="str">
-        <v>2021-06-21 00:00:00</v>
+        <v>2021-06-23 00:00:00</v>
       </c>
     </row>
     <row r="4">
@@ -499,37 +499,37 @@
         <v>2</v>
       </c>
       <c r="B4">
-        <v>7298</v>
+        <v>0</v>
       </c>
       <c r="C4">
-        <v>4868</v>
+        <v>0</v>
       </c>
       <c r="D4">
-        <v>4602</v>
+        <v>0</v>
       </c>
       <c r="E4">
-        <v>4687</v>
+        <v>0</v>
       </c>
       <c r="F4">
-        <v>4667</v>
+        <v>0</v>
       </c>
       <c r="G4">
-        <v>5139</v>
+        <v>0</v>
       </c>
       <c r="H4">
-        <v>4493</v>
+        <v>0</v>
       </c>
       <c r="I4">
-        <v>5116</v>
+        <v>0</v>
       </c>
       <c r="J4">
-        <v>4952</v>
+        <v>0</v>
       </c>
       <c r="K4">
-        <v>4909</v>
+        <v>0</v>
       </c>
       <c r="L4" t="str">
-        <v>2021-06-20 00:00:00</v>
+        <v>2021-06-22 00:00:00</v>
       </c>
     </row>
     <row r="5">
@@ -537,37 +537,37 @@
         <v>3</v>
       </c>
       <c r="B5">
-        <v>7463</v>
+        <v>0</v>
       </c>
       <c r="C5">
-        <v>4694</v>
+        <v>0</v>
       </c>
       <c r="D5">
-        <v>4576</v>
+        <v>0</v>
       </c>
       <c r="E5">
-        <v>4863</v>
+        <v>0</v>
       </c>
       <c r="F5">
-        <v>4610</v>
+        <v>0</v>
       </c>
       <c r="G5">
-        <v>4940</v>
+        <v>0</v>
       </c>
       <c r="H5">
-        <v>4765</v>
+        <v>0</v>
       </c>
       <c r="I5">
-        <v>4431</v>
+        <v>0</v>
       </c>
       <c r="J5">
-        <v>4377</v>
+        <v>0</v>
       </c>
       <c r="K5">
-        <v>4838</v>
+        <v>0</v>
       </c>
       <c r="L5" t="str">
-        <v>2021-06-19 00:00:00</v>
+        <v>2021-06-21 00:00:00</v>
       </c>
     </row>
     <row r="6">
@@ -575,37 +575,37 @@
         <v>4</v>
       </c>
       <c r="B6">
-        <v>7661</v>
+        <v>0</v>
       </c>
       <c r="C6">
-        <v>4431</v>
+        <v>0</v>
       </c>
       <c r="D6">
-        <v>4492</v>
+        <v>0</v>
       </c>
       <c r="E6">
-        <v>4495</v>
+        <v>0</v>
       </c>
       <c r="F6">
-        <v>5380</v>
+        <v>0</v>
       </c>
       <c r="G6">
-        <v>5070</v>
+        <v>0</v>
       </c>
       <c r="H6">
-        <v>4813</v>
+        <v>0</v>
       </c>
       <c r="I6">
-        <v>4749</v>
+        <v>0</v>
       </c>
       <c r="J6">
-        <v>4878</v>
+        <v>0</v>
       </c>
       <c r="K6">
-        <v>5122</v>
+        <v>0</v>
       </c>
       <c r="L6" t="str">
-        <v>2021-06-18 00:00:00</v>
+        <v>2021-06-20 00:00:00</v>
       </c>
     </row>
     <row r="7">
@@ -613,37 +613,37 @@
         <v>5</v>
       </c>
       <c r="B7">
-        <v>13413</v>
+        <v>0</v>
       </c>
       <c r="C7">
-        <v>7803</v>
+        <v>0</v>
       </c>
       <c r="D7">
-        <v>7715</v>
+        <v>0</v>
       </c>
       <c r="E7">
-        <v>8017</v>
+        <v>0</v>
       </c>
       <c r="F7">
-        <v>8192</v>
+        <v>0</v>
       </c>
       <c r="G7">
-        <v>8613</v>
+        <v>0</v>
       </c>
       <c r="H7">
-        <v>8462</v>
+        <v>0</v>
       </c>
       <c r="I7">
-        <v>8194</v>
+        <v>0</v>
       </c>
       <c r="J7">
-        <v>7987</v>
+        <v>0</v>
       </c>
       <c r="K7">
-        <v>7976</v>
+        <v>0</v>
       </c>
       <c r="L7" t="str">
-        <v>2021-06-17 00:00:00</v>
+        <v>2021-06-19 00:00:00</v>
       </c>
     </row>
     <row r="8">
@@ -651,37 +651,37 @@
         <v>6</v>
       </c>
       <c r="B8">
-        <v>14055</v>
+        <v>0</v>
       </c>
       <c r="C8">
-        <v>8600</v>
+        <v>0</v>
       </c>
       <c r="D8">
-        <v>7915</v>
+        <v>0</v>
       </c>
       <c r="E8">
-        <v>7845</v>
+        <v>0</v>
       </c>
       <c r="F8">
-        <v>8317</v>
+        <v>0</v>
       </c>
       <c r="G8">
-        <v>8414</v>
+        <v>0</v>
       </c>
       <c r="H8">
-        <v>7527</v>
+        <v>0</v>
       </c>
       <c r="I8">
-        <v>8192</v>
+        <v>0</v>
       </c>
       <c r="J8">
-        <v>7249</v>
+        <v>0</v>
       </c>
       <c r="K8">
-        <v>8261</v>
+        <v>0</v>
       </c>
       <c r="L8" t="str">
-        <v>2021-06-16 00:00:00</v>
+        <v>2021-06-18 00:00:00</v>
       </c>
     </row>
   </sheetData>

</xml_diff>